<commit_message>
Format Key Metrics Values on Dashboard.
</commit_message>
<xml_diff>
--- a/interface/project_data/generated_data/users.xlsx
+++ b/interface/project_data/generated_data/users.xlsx
@@ -636,43 +636,43 @@
         <v>5</v>
       </c>
       <c r="D4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O4" t="n">
         <v>5</v>
       </c>
-      <c r="E4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="L4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2.5</v>
-      </c>
       <c r="P4" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="Q4" t="n">
         <v>2.5</v>
@@ -681,7 +681,7 @@
         <v>2.5</v>
       </c>
       <c r="S4" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fix issue with new user skills and skill comparison.
</commit_message>
<xml_diff>
--- a/interface/project_data/generated_data/users.xlsx
+++ b/interface/project_data/generated_data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,152 +436,157 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Adaptability</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Computers and information technology</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Creativity</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Critical and Analytical Thinking</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Customer Service</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Detail Oriented</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Fine Motor Skills</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Interpersonal Relations</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Leadership</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Mechanical</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Physical Strength and Stamina</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Problem Solving and Decision Making</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Project Management</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Scientific Skills</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Speaking and Listening</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Writing and Reading</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Added Skills</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Atharv</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
       <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
         <v>4.5</v>
       </c>
-      <c r="D2" t="n">
-        <v>5</v>
-      </c>
       <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
         <v>4</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>4.5</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>3.5</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>4</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>3.5</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4</v>
       </c>
       <c r="K2" t="n">
         <v>4</v>
       </c>
       <c r="L2" t="n">
+        <v>4</v>
+      </c>
+      <c r="M2" t="n">
         <v>4.5</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>4</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>3.5</v>
-      </c>
-      <c r="O2" t="n">
-        <v>4</v>
       </c>
       <c r="P2" t="n">
         <v>4</v>
@@ -590,20 +595,25 @@
         <v>4</v>
       </c>
       <c r="R2" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="S2" t="n">
         <v>4.5</v>
       </c>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>AP</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -622,25 +632,26 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AA</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
       <c r="C4" t="n">
         <v>5</v>
       </c>
       <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
         <v>4.5</v>
       </c>
-      <c r="E4" t="n">
-        <v>2.5</v>
-      </c>
       <c r="F4" t="n">
         <v>2.5</v>
       </c>
@@ -669,33 +680,34 @@
         <v>2.5</v>
       </c>
       <c r="O4" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="P4" t="n">
         <v>5</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="R4" t="n">
         <v>2.5</v>
       </c>
       <c r="S4" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Test1</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>2.5</v>
-      </c>
       <c r="C5" t="n">
         <v>2.5</v>
       </c>
@@ -748,16 +760,19 @@
         <v>2.5</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Diya</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -776,6 +791,72 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="T7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="U7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Occupation Selection on Sign up
</commit_message>
<xml_diff>
--- a/interface/project_data/generated_data/users.xlsx
+++ b/interface/project_data/generated_data/users.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,162 +434,162 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Adaptability</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Computers and information technology</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Creativity</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Critical and Analytical Thinking</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Customer Service</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Detail Oriented</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fine Motor Skills</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Interpersonal Relations</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Leadership</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Mechanical</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Physical Strength and Stamina</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Problem Solving and Decision Making</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Project Management</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Scientific Skills</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Speaking and Listening</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Writing and Reading</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Added Skills</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Atharv</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
       <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
         <v>4.5</v>
       </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
       <c r="F2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" t="n">
         <v>4</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>4.5</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>3.5</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>4</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>3.5</v>
-      </c>
-      <c r="K2" t="n">
-        <v>4</v>
       </c>
       <c r="L2" t="n">
         <v>4</v>
       </c>
       <c r="M2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N2" t="n">
         <v>4.5</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>4</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>3.5</v>
-      </c>
-      <c r="P2" t="n">
-        <v>4</v>
       </c>
       <c r="Q2" t="n">
         <v>4</v>
@@ -598,23 +598,28 @@
         <v>4</v>
       </c>
       <c r="S2" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="T2" t="n">
         <v>4.5</v>
       </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>AP</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -633,28 +638,29 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>AA</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
       <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
         <v>4.5</v>
       </c>
-      <c r="F4" t="n">
-        <v>2.5</v>
-      </c>
       <c r="G4" t="n">
         <v>2.5</v>
       </c>
@@ -683,34 +689,37 @@
         <v>2.5</v>
       </c>
       <c r="P4" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="Q4" t="n">
         <v>5</v>
       </c>
       <c r="R4" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="S4" t="n">
         <v>2.5</v>
       </c>
       <c r="T4" t="n">
-        <v>5</v>
-      </c>
-      <c r="U4" t="inlineStr"/>
+        <v>2.5</v>
+      </c>
+      <c r="U4" t="n">
+        <v>5</v>
+      </c>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Test1</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>2.5</v>
-      </c>
       <c r="D5" t="n">
         <v>2.5</v>
       </c>
@@ -762,18 +771,23 @@
       <c r="T5" t="n">
         <v>2.5</v>
       </c>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>Diya</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -792,27 +806,28 @@
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
       <c r="D7" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="F7" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
         <v>2.5</v>
@@ -830,13 +845,13 @@
         <v>2.5</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="M7" t="n">
         <v>5</v>
       </c>
       <c r="N7" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="O7" t="n">
         <v>2.5</v>
@@ -856,7 +871,40 @@
       <c r="T7" t="n">
         <v>2.5</v>
       </c>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="V7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>KS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>